<commit_message>
fix: corrige validação de data
</commit_message>
<xml_diff>
--- a/input/piu-monitoramento_v2.xlsx
+++ b/input/piu-monitoramento_v2.xlsx
@@ -15392,12 +15392,12 @@
         <f>IFERROR(VLOOKUP(C190,tramitacao!$A$2:$B$101,2,0),"0")</f>
         <v>Consulta Pública Inicial</v>
       </c>
-      <c r="E190" s="10">
-        <v>0.0</v>
+      <c r="E190" s="4">
+        <v>2.0</v>
       </c>
       <c r="F190" s="2" t="str">
         <f>IFERROR(VLOOKUP(E190,grupos!$A$2:$B$100,2,0),"0")</f>
-        <v>0</v>
+        <v>Consulta Inicial</v>
       </c>
       <c r="G190" s="10">
         <v>1.0</v>
@@ -24602,12 +24602,12 @@
         <f>IFERROR(VLOOKUP(C420,tramitacao!$A$2:$B$101,2,0),"0")</f>
         <v>Proposição</v>
       </c>
-      <c r="E420" s="10">
-        <v>0.0</v>
+      <c r="E420" s="4">
+        <v>8.0</v>
       </c>
       <c r="F420" s="2" t="str">
         <f>IFERROR(VLOOKUP(E420,grupos!$A$2:$B$100,2,0),"0")</f>
-        <v>0</v>
+        <v>Processo Administrativo</v>
       </c>
       <c r="G420" s="10">
         <v>11.0</v>
@@ -24642,12 +24642,12 @@
         <f>IFERROR(VLOOKUP(C421,tramitacao!$A$2:$B$101,2,0),"0")</f>
         <v>Proposição</v>
       </c>
-      <c r="E421" s="10">
-        <v>0.0</v>
+      <c r="E421" s="4">
+        <v>8.0</v>
       </c>
       <c r="F421" s="2" t="str">
         <f>IFERROR(VLOOKUP(E421,grupos!$A$2:$B$100,2,0),"0")</f>
-        <v>0</v>
+        <v>Processo Administrativo</v>
       </c>
       <c r="G421" s="10">
         <v>11.0</v>
@@ -24762,12 +24762,12 @@
         <f>IFERROR(VLOOKUP(C424,tramitacao!$A$2:$B$101,2,0),"0")</f>
         <v>Proposição</v>
       </c>
-      <c r="E424" s="10">
-        <v>0.0</v>
+      <c r="E424" s="4">
+        <v>8.0</v>
       </c>
       <c r="F424" s="2" t="str">
         <f>IFERROR(VLOOKUP(E424,grupos!$A$2:$B$100,2,0),"0")</f>
-        <v>0</v>
+        <v>Processo Administrativo</v>
       </c>
       <c r="G424" s="10">
         <v>13.0</v>
@@ -31992,12 +31992,12 @@
         <f>IFERROR(VLOOKUP(C595,tramitacao!$A$2:$B$101,2,0),"0")</f>
         <v>Avaliação SMUL</v>
       </c>
-      <c r="E595" s="10">
-        <v>0.0</v>
+      <c r="E595" s="4">
+        <v>6.0</v>
       </c>
       <c r="F595" s="2" t="str">
         <f>IFERROR(VLOOKUP(E595,grupos!$A$2:$B$100,2,0),"0")</f>
-        <v>0</v>
+        <v>Outros</v>
       </c>
       <c r="G595" s="10">
         <v>21.0</v>

</xml_diff>